<commit_message>
AMOVA - isolation by distance - allele frequencies
</commit_message>
<xml_diff>
--- a/Koordinaten_2024.xlsx
+++ b/Koordinaten_2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wslch365-my.sharepoint.com/personal/lia_baumann_wsl_ch/Documents/R/truffles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{53E3C729-3A50-4BC6-A70C-A9EE5E16EAC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29472BC9-83DD-419E-922B-8FF60BB364DA}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{53E3C729-3A50-4BC6-A70C-A9EE5E16EAC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0E9B930-7DD3-4E22-8877-A68C5528BAFD}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="77490" yWindow="0" windowWidth="17415" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -237,6 +237,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -529,7 +533,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -936,6 +940,15 @@
       </c>
       <c r="B24" t="s">
         <v>49</v>
+      </c>
+      <c r="C24">
+        <v>52.375900000000001</v>
+      </c>
+      <c r="D24">
+        <v>9.7319999999999993</v>
+      </c>
+      <c r="E24">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>